<commit_message>
New changes by openpyxl
</commit_message>
<xml_diff>
--- a/sheet.xlsx
+++ b/sheet.xlsx
@@ -29,12 +29,17 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF0000"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -60,12 +65,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -442,7 +448,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 0</t>
+          <t>Unnamed: 0.1</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -509,127 +515,137 @@
           <t>This course is related to programming</t>
         </is>
       </c>
-      <c r="H2" s="2" t="inlineStr"/>
+      <c r="H2" s="2" t="n">
+        <v>45</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="n">
+      <c r="A3" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="n">
+      <c r="B3" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="inlineStr">
+      <c r="C3" s="3" t="inlineStr">
         <is>
           <t>adnan</t>
         </is>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="D3" s="3" t="n">
         <v>90</v>
       </c>
-      <c r="E3" s="2" t="n">
+      <c r="E3" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="F3" s="2" t="inlineStr">
+      <c r="F3" s="3" t="inlineStr">
         <is>
           <t>Distributed Programming</t>
         </is>
       </c>
-      <c r="G3" s="2" t="inlineStr">
+      <c r="G3" s="3" t="inlineStr">
         <is>
           <t>This course is related to programming</t>
         </is>
       </c>
-      <c r="H3" s="2" t="inlineStr"/>
+      <c r="H3" s="3" t="n">
+        <v>90</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="n">
+      <c r="A4" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="n">
+      <c r="B4" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="inlineStr">
+      <c r="C4" s="3" t="inlineStr">
         <is>
           <t>Kashif</t>
         </is>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D4" s="3" t="n">
         <v>85</v>
       </c>
-      <c r="E4" s="2" t="n">
+      <c r="E4" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="F4" s="2" t="inlineStr">
+      <c r="F4" s="3" t="inlineStr">
         <is>
           <t>networking</t>
         </is>
       </c>
-      <c r="G4" s="2" t="inlineStr">
+      <c r="G4" s="3" t="inlineStr">
         <is>
           <t>This course is related to Networking</t>
         </is>
       </c>
-      <c r="H4" s="2" t="inlineStr"/>
+      <c r="H4" s="3" t="n">
+        <v>85</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="n">
+      <c r="A5" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="C5" s="2" t="inlineStr">
+      <c r="C5" s="3" t="inlineStr">
         <is>
           <t>wardha</t>
         </is>
       </c>
-      <c r="D5" s="2" t="n">
+      <c r="D5" s="3" t="n">
         <v>67</v>
       </c>
-      <c r="E5" s="2" t="n">
+      <c r="E5" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="F5" s="2" t="inlineStr">
+      <c r="F5" s="3" t="inlineStr">
         <is>
           <t>Databases</t>
         </is>
       </c>
-      <c r="G5" s="2" t="inlineStr">
+      <c r="G5" s="3" t="inlineStr">
         <is>
           <t>This course is related to Databases</t>
         </is>
       </c>
-      <c r="H5" s="2" t="inlineStr"/>
+      <c r="H5" s="3" t="n">
+        <v>67</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="n">
+      <c r="A6" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="C6" s="2" t="inlineStr">
+      <c r="C6" s="3" t="inlineStr">
         <is>
           <t>Kashif</t>
         </is>
       </c>
-      <c r="D6" s="2" t="n">
+      <c r="D6" s="3" t="n">
         <v>88</v>
       </c>
-      <c r="E6" s="2" t="n">
+      <c r="E6" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="F6" s="2" t="inlineStr">
+      <c r="F6" s="3" t="inlineStr">
         <is>
           <t>DSA</t>
         </is>
       </c>
-      <c r="G6" s="2" t="inlineStr">
+      <c r="G6" s="3" t="inlineStr">
         <is>
           <t>This course is related to DSA</t>
         </is>
       </c>
-      <c r="H6" s="2" t="inlineStr"/>
+      <c r="H6" s="3" t="n">
+        <v>88</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>